<commit_message>
ukrainian translation fix (#49)
</commit_message>
<xml_diff>
--- a/i18n/uk.xlsx
+++ b/i18n/uk.xlsx
@@ -1279,7 +1279,7 @@
     <t xml:space="preserve">Parus major</t>
   </si>
   <si>
-    <t xml:space="preserve">Синиця велика </t>
+    <t xml:space="preserve">Синиця велика</t>
   </si>
   <si>
     <t xml:space="preserve">Оновити годівницю. Якщо зробили це, отримайте 1 [die] з годівниці після оновлення.</t>
@@ -4915,9 +4915,9 @@
   <dimension ref="A1:J364"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A338" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A201" activeCellId="0" sqref="A201"/>
+      <selection pane="bottomLeft" activeCell="D138" activeCellId="0" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4928,7 +4928,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="45.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="116.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>